<commit_message>
real HW to TROS
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2725" uniqueCount="89">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -213,6 +213,75 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;v&gt; : &lt;v&gt;543</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upcdl.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZWAdobeF.TTF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAL : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAL : &lt;v&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ariblk.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAL : &lt;v&gt;&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAL : &lt;v&gt;&lt;v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,a-z,A-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234567890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResourceId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
   </si>
 </sst>
 </file>
@@ -1441,7 +1510,7 @@
         <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -1532,6 +1601,26 @@
       <c r="O6" s="11"/>
     </row>
     <row r="7" spans="2:15">
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7"/>
       <c r="K7" s="8" t="s">
         <v>15</v>
       </c>
@@ -1680,16 +1769,16 @@
     </row>
     <row r="4" spans="2:10" ht="15" customHeight="1">
       <c r="B4" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
         <v>50</v>
@@ -1697,7 +1786,7 @@
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
       <c r="B5" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
         <v>42</v>
@@ -1706,14 +1795,46 @@
         <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="2:10"/>
-    <row r="7" spans="2:10"/>
+    <row r="6" spans="2:10">
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="8" spans="2:10"/>
     <row r="9" spans="2:10"/>
     <row r="10" spans="2:10"/>

</xml_diff>

<commit_message>
main screen finish updateTime();
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49861" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54126" uniqueCount="278">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2823,7 +2823,7 @@
         <v>49</v>
       </c>
       <c r="E26" t="s">
-        <v>263</v>
+        <v>129</v>
       </c>
       <c r="F26" t="s">
         <v>50</v>
@@ -2840,7 +2840,7 @@
         <v>49</v>
       </c>
       <c r="E27" t="s">
-        <v>264</v>
+        <v>132</v>
       </c>
       <c r="F27" t="s">
         <v>50</v>
@@ -2857,7 +2857,7 @@
         <v>49</v>
       </c>
       <c r="E28" t="s">
-        <v>265</v>
+        <v>134</v>
       </c>
       <c r="F28" t="s">
         <v>50</v>
@@ -2874,7 +2874,7 @@
         <v>49</v>
       </c>
       <c r="E29" t="s">
-        <v>266</v>
+        <v>136</v>
       </c>
       <c r="F29" t="s">
         <v>50</v>
@@ -2891,7 +2891,7 @@
         <v>49</v>
       </c>
       <c r="E30" t="s">
-        <v>267</v>
+        <v>140</v>
       </c>
       <c r="F30" t="s">
         <v>50</v>
@@ -2908,7 +2908,7 @@
         <v>49</v>
       </c>
       <c r="E31" t="s">
-        <v>268</v>
+        <v>143</v>
       </c>
       <c r="F31" t="s">
         <v>50</v>
@@ -2925,7 +2925,7 @@
         <v>49</v>
       </c>
       <c r="E32" t="s">
-        <v>269</v>
+        <v>146</v>
       </c>
       <c r="F32" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
finish Calendar & swap by function
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54126" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73357" uniqueCount="294">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -849,6 +849,54 @@
   </si>
   <si>
     <t xml:space="preserve">a-z,A-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YEAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUMID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;V&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;V&gt;%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;v&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-z,A-Z,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-z,A-Z,0-9</t>
   </si>
 </sst>
 </file>
@@ -2189,7 +2237,7 @@
       </c>
       <c r="G7"/>
       <c r="H7" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="I7"/>
       <c r="K7" s="8" t="s">
@@ -2224,7 +2272,9 @@
       <c r="F8" t="s">
         <v>25</v>
       </c>
-      <c r="G8"/>
+      <c r="G8" t="s">
+        <v>288</v>
+      </c>
       <c r="H8" t="s">
         <v>80</v>
       </c>
@@ -2670,7 +2720,7 @@
         <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>119</v>
+        <v>281</v>
       </c>
       <c r="F17" t="s">
         <v>50</v>
@@ -4750,11 +4800,91 @@
         <v>50</v>
       </c>
     </row>
-    <row r="140" spans="4:4"/>
-    <row r="141" spans="4:4"/>
-    <row r="142" spans="4:4"/>
-    <row r="143" spans="4:4"/>
-    <row r="144" spans="4:4"/>
+    <row r="140" spans="4:4">
+      <c r="B140" t="s">
+        <v>278</v>
+      </c>
+      <c r="C140" t="s">
+        <v>42</v>
+      </c>
+      <c r="D140" t="s">
+        <v>49</v>
+      </c>
+      <c r="E140" t="s">
+        <v>119</v>
+      </c>
+      <c r="F140" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="141" spans="4:4">
+      <c r="B141" t="s">
+        <v>279</v>
+      </c>
+      <c r="C141" t="s">
+        <v>42</v>
+      </c>
+      <c r="D141" t="s">
+        <v>49</v>
+      </c>
+      <c r="E141" t="s">
+        <v>283</v>
+      </c>
+      <c r="F141" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="142" spans="4:4">
+      <c r="B142" t="s">
+        <v>284</v>
+      </c>
+      <c r="C142" t="s">
+        <v>100</v>
+      </c>
+      <c r="D142" t="s">
+        <v>103</v>
+      </c>
+      <c r="E142" t="s">
+        <v>290</v>
+      </c>
+      <c r="F142" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="143" spans="4:4">
+      <c r="B143" t="s">
+        <v>289</v>
+      </c>
+      <c r="C143" t="s">
+        <v>42</v>
+      </c>
+      <c r="D143" t="s">
+        <v>49</v>
+      </c>
+      <c r="E143" t="s">
+        <v>288</v>
+      </c>
+      <c r="F143" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="144" spans="4:4">
+      <c r="B144" t="s">
+        <v>291</v>
+      </c>
+      <c r="C144" t="s">
+        <v>100</v>
+      </c>
+      <c r="D144" t="s">
+        <v>49</v>
+      </c>
+      <c r="E144" t="s">
+        <v>79</v>
+      </c>
+      <c r="F144" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="145" spans="4:4"/>
     <row r="146" spans="4:4"/>
     <row r="147" spans="4:4"/>

</xml_diff>

<commit_message>
update screen 0 and 1 ->button , cnt_up building
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73357" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75095" uniqueCount="294">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -4411,7 +4411,7 @@
     </row>
     <row r="117" spans="4:4">
       <c r="B117" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C117" t="s">
         <v>43</v>
@@ -4428,7 +4428,7 @@
     </row>
     <row r="118" spans="4:4">
       <c r="B118" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C118" t="s">
         <v>43</v>
@@ -4445,7 +4445,7 @@
     </row>
     <row r="119" spans="4:4">
       <c r="B119" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="C119" t="s">
         <v>43</v>
@@ -4462,13 +4462,13 @@
     </row>
     <row r="120" spans="4:4">
       <c r="B120" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="C120" t="s">
         <v>43</v>
       </c>
       <c r="D120" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="E120" t="s">
         <v>95</v>
@@ -4479,7 +4479,7 @@
     </row>
     <row r="121" spans="4:4">
       <c r="B121" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="C121" t="s">
         <v>43</v>
@@ -4496,16 +4496,16 @@
     </row>
     <row r="122" spans="4:4">
       <c r="B122" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="C122" t="s">
-        <v>43</v>
+        <v>255</v>
       </c>
       <c r="D122" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="E122" t="s">
-        <v>95</v>
+        <v>256</v>
       </c>
       <c r="F122" t="s">
         <v>50</v>
@@ -4513,16 +4513,16 @@
     </row>
     <row r="123" spans="4:4">
       <c r="B123" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C123" t="s">
         <v>43</v>
       </c>
       <c r="D123" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="E123" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F123" t="s">
         <v>50</v>
@@ -4530,7 +4530,7 @@
     </row>
     <row r="124" spans="4:4">
       <c r="B124" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="C124" t="s">
         <v>43</v>
@@ -4539,7 +4539,7 @@
         <v>49</v>
       </c>
       <c r="E124" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="F124" t="s">
         <v>50</v>
@@ -4547,16 +4547,16 @@
     </row>
     <row r="125" spans="4:4">
       <c r="B125" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="C125" t="s">
         <v>43</v>
       </c>
       <c r="D125" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="E125" t="s">
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="F125" t="s">
         <v>50</v>
@@ -4564,16 +4564,16 @@
     </row>
     <row r="126" spans="4:4">
       <c r="B126" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="C126" t="s">
         <v>43</v>
       </c>
       <c r="D126" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="E126" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F126" t="s">
         <v>50</v>
@@ -4581,16 +4581,16 @@
     </row>
     <row r="127" spans="4:4">
       <c r="B127" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="C127" t="s">
-        <v>255</v>
+        <v>43</v>
       </c>
       <c r="D127" t="s">
         <v>49</v>
       </c>
       <c r="E127" t="s">
-        <v>256</v>
+        <v>97</v>
       </c>
       <c r="F127" t="s">
         <v>50</v>
@@ -4598,16 +4598,16 @@
     </row>
     <row r="128" spans="4:4">
       <c r="B128" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="C128" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D128" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="E128" t="s">
-        <v>95</v>
+        <v>262</v>
       </c>
       <c r="F128" t="s">
         <v>50</v>
@@ -4615,16 +4615,16 @@
     </row>
     <row r="129" spans="4:4">
       <c r="B129" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="C129" t="s">
         <v>43</v>
       </c>
       <c r="D129" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="E129" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F129" t="s">
         <v>50</v>
@@ -4632,7 +4632,7 @@
     </row>
     <row r="130" spans="4:4">
       <c r="B130" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="C130" t="s">
         <v>43</v>
@@ -4641,7 +4641,7 @@
         <v>49</v>
       </c>
       <c r="E130" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="F130" t="s">
         <v>50</v>
@@ -4649,16 +4649,16 @@
     </row>
     <row r="131" spans="4:4">
       <c r="B131" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="C131" t="s">
         <v>43</v>
       </c>
       <c r="D131" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="E131" t="s">
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="F131" t="s">
         <v>50</v>
@@ -4666,16 +4666,16 @@
     </row>
     <row r="132" spans="4:4">
       <c r="B132" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="C132" t="s">
         <v>43</v>
       </c>
       <c r="D132" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="E132" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F132" t="s">
         <v>50</v>
@@ -4683,16 +4683,16 @@
     </row>
     <row r="133" spans="4:4">
       <c r="B133" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="C133" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D133" t="s">
         <v>49</v>
       </c>
       <c r="E133" t="s">
-        <v>262</v>
+        <v>97</v>
       </c>
       <c r="F133" t="s">
         <v>50</v>
@@ -4700,16 +4700,16 @@
     </row>
     <row r="134" spans="4:4">
       <c r="B134" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="C134" t="s">
-        <v>43</v>
+        <v>255</v>
       </c>
       <c r="D134" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="E134" t="s">
-        <v>95</v>
+        <v>256</v>
       </c>
       <c r="F134" t="s">
         <v>50</v>
@@ -4717,16 +4717,16 @@
     </row>
     <row r="135" spans="4:4">
       <c r="B135" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="C135" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D135" t="s">
         <v>49</v>
       </c>
       <c r="E135" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="F135" t="s">
         <v>50</v>
@@ -4734,16 +4734,16 @@
     </row>
     <row r="136" spans="4:4">
       <c r="B136" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="C136" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D136" t="s">
         <v>49</v>
       </c>
       <c r="E136" t="s">
-        <v>56</v>
+        <v>283</v>
       </c>
       <c r="F136" t="s">
         <v>50</v>
@@ -4751,16 +4751,16 @@
     </row>
     <row r="137" spans="4:4">
       <c r="B137" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="C137" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="D137" t="s">
         <v>103</v>
       </c>
       <c r="E137" t="s">
-        <v>95</v>
+        <v>290</v>
       </c>
       <c r="F137" t="s">
         <v>50</v>
@@ -4768,16 +4768,16 @@
     </row>
     <row r="138" spans="4:4">
       <c r="B138" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="C138" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D138" t="s">
         <v>49</v>
       </c>
       <c r="E138" t="s">
-        <v>97</v>
+        <v>288</v>
       </c>
       <c r="F138" t="s">
         <v>50</v>
@@ -4785,106 +4785,26 @@
     </row>
     <row r="139" spans="4:4">
       <c r="B139" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="C139" t="s">
-        <v>255</v>
+        <v>100</v>
       </c>
       <c r="D139" t="s">
         <v>49</v>
       </c>
       <c r="E139" t="s">
-        <v>256</v>
+        <v>79</v>
       </c>
       <c r="F139" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="140" spans="4:4">
-      <c r="B140" t="s">
-        <v>278</v>
-      </c>
-      <c r="C140" t="s">
-        <v>42</v>
-      </c>
-      <c r="D140" t="s">
-        <v>49</v>
-      </c>
-      <c r="E140" t="s">
-        <v>119</v>
-      </c>
-      <c r="F140" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="141" spans="4:4">
-      <c r="B141" t="s">
-        <v>279</v>
-      </c>
-      <c r="C141" t="s">
-        <v>42</v>
-      </c>
-      <c r="D141" t="s">
-        <v>49</v>
-      </c>
-      <c r="E141" t="s">
-        <v>283</v>
-      </c>
-      <c r="F141" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="142" spans="4:4">
-      <c r="B142" t="s">
-        <v>284</v>
-      </c>
-      <c r="C142" t="s">
-        <v>100</v>
-      </c>
-      <c r="D142" t="s">
-        <v>103</v>
-      </c>
-      <c r="E142" t="s">
-        <v>290</v>
-      </c>
-      <c r="F142" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="143" spans="4:4">
-      <c r="B143" t="s">
-        <v>289</v>
-      </c>
-      <c r="C143" t="s">
-        <v>42</v>
-      </c>
-      <c r="D143" t="s">
-        <v>49</v>
-      </c>
-      <c r="E143" t="s">
-        <v>288</v>
-      </c>
-      <c r="F143" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="144" spans="4:4">
-      <c r="B144" t="s">
-        <v>291</v>
-      </c>
-      <c r="C144" t="s">
-        <v>100</v>
-      </c>
-      <c r="D144" t="s">
-        <v>49</v>
-      </c>
-      <c r="E144" t="s">
-        <v>79</v>
-      </c>
-      <c r="F144" t="s">
-        <v>50</v>
-      </c>
-    </row>
+    <row r="140" spans="4:4"/>
+    <row r="141" spans="4:4"/>
+    <row r="142" spans="4:4"/>
+    <row r="143" spans="4:4"/>
+    <row r="144" spans="4:4"/>
     <row r="145" spans="4:4"/>
     <row r="146" spans="4:4"/>
     <row r="147" spans="4:4"/>

</xml_diff>